<commit_message>
Spread sheet format changes
Added / to mapped pin names where there are multiple mapped min names
for the same pin
</commit_message>
<xml_diff>
--- a/M2 Pin Mapping.xlsx
+++ b/M2 Pin Mapping.xlsx
@@ -1063,9 +1063,6 @@
     <t>SPI0_CS1</t>
   </si>
   <si>
-    <t>PS_BUCK  BUCK_DIS</t>
-  </si>
-  <si>
     <t>PS_J1850_9141</t>
   </si>
   <si>
@@ -1078,12 +1075,6 @@
     <t>J1850N_TX</t>
   </si>
   <si>
-    <t>CAN0_CS  HS_CS</t>
-  </si>
-  <si>
-    <t>CAN1_CS  MS_CS</t>
-  </si>
-  <si>
     <t>I_SENSE_EN</t>
   </si>
   <si>
@@ -1117,9 +1108,6 @@
     <t>CPU Test Point</t>
   </si>
   <si>
-    <t>CPU_TEMP  A15</t>
-  </si>
-  <si>
     <t>GPIO Power Supply Analog Current Sense</t>
   </si>
   <si>
@@ -1910,6 +1898,18 @@
   </si>
   <si>
     <t>Power Supply</t>
+  </si>
+  <si>
+    <t>CAN0_CS / HS_CS</t>
+  </si>
+  <si>
+    <t>CAN1_CS / MS_CS</t>
+  </si>
+  <si>
+    <t>CPU_TEMP / A15</t>
+  </si>
+  <si>
+    <t>PS_BUCK / BUCK_DIS</t>
   </si>
 </sst>
 </file>
@@ -2359,6 +2359,45 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2366,24 +2405,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2420,27 +2441,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2729,8 +2729,8 @@
   <dimension ref="A1:AJ352"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2745,25 +2745,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="95" t="s">
-        <v>357</v>
-      </c>
-      <c r="F1" s="95" t="s">
+      <c r="E1" s="74" t="s">
+        <v>354</v>
+      </c>
+      <c r="F1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="93" t="s">
+      <c r="G1" s="72" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2771,7 +2771,7 @@
       <c r="A2" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="90">
+      <c r="B2" s="69">
         <v>14</v>
       </c>
       <c r="C2" s="68" t="s">
@@ -2780,11 +2780,11 @@
       <c r="D2" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="91" t="s">
+      <c r="E2" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="91"/>
-      <c r="G2" s="92">
+      <c r="F2" s="70"/>
+      <c r="G2" s="71">
         <v>32</v>
       </c>
       <c r="H2" s="19"/>
@@ -3192,7 +3192,7 @@
       <c r="AJ10" s="20"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="85" t="s">
         <v>321</v>
       </c>
       <c r="B11" s="34">
@@ -3208,7 +3208,7 @@
         <v>21</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="G11" s="4">
         <v>138</v>
@@ -3244,7 +3244,7 @@
       <c r="AJ11" s="19"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12" s="78"/>
+      <c r="A12" s="85"/>
       <c r="B12" s="34">
         <v>23</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>23</v>
       </c>
       <c r="F12" s="64" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="G12" s="4">
         <v>121</v>
@@ -3332,8 +3332,8 @@
       <c r="AJ13" s="20"/>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A14" s="75" t="s">
-        <v>399</v>
+      <c r="A14" s="78" t="s">
+        <v>395</v>
       </c>
       <c r="B14" s="37">
         <v>36</v>
@@ -3710,8 +3710,8 @@
       <c r="AJ21" s="20"/>
     </row>
     <row r="22" spans="1:36" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="75" t="s">
-        <v>400</v>
+      <c r="A22" s="78" t="s">
+        <v>396</v>
       </c>
       <c r="B22" s="37">
         <f>B101</f>
@@ -3962,7 +3962,7 @@
       <c r="AJ26" s="20"/>
     </row>
     <row r="27" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A27" s="72" t="s">
+      <c r="A27" s="79" t="s">
         <v>40</v>
       </c>
       <c r="B27" s="34">
@@ -3972,13 +3972,13 @@
         <v>322</v>
       </c>
       <c r="D27" s="33" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="E27" s="32" t="s">
         <v>41</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="G27" s="4">
         <v>60</v>
@@ -4014,7 +4014,7 @@
       <c r="AJ27" s="19"/>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A28" s="73"/>
+      <c r="A28" s="81"/>
       <c r="B28" s="34">
         <v>25</v>
       </c>
@@ -4022,13 +4022,13 @@
         <v>323</v>
       </c>
       <c r="D28" s="33" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="E28" s="32" t="s">
         <v>43</v>
       </c>
       <c r="F28" s="32" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="G28" s="4">
         <v>63</v>
@@ -4064,7 +4064,7 @@
       <c r="AJ28" s="19"/>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A29" s="73"/>
+      <c r="A29" s="81"/>
       <c r="B29" s="34">
         <v>26</v>
       </c>
@@ -4072,13 +4072,13 @@
         <v>324</v>
       </c>
       <c r="D29" s="33" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="E29" s="32" t="s">
         <v>45</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="G29" s="4">
         <v>65</v>
@@ -4114,7 +4114,7 @@
       <c r="AJ29" s="19"/>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A30" s="73"/>
+      <c r="A30" s="81"/>
       <c r="B30" s="34">
         <v>27</v>
       </c>
@@ -4122,13 +4122,13 @@
         <v>325</v>
       </c>
       <c r="D30" s="33" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="E30" s="32" t="s">
         <v>47</v>
       </c>
       <c r="F30" s="32" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="G30" s="4">
         <v>67</v>
@@ -4164,7 +4164,7 @@
       <c r="AJ30" s="19"/>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A31" s="73"/>
+      <c r="A31" s="81"/>
       <c r="B31" s="34">
         <v>28</v>
       </c>
@@ -4172,13 +4172,13 @@
         <v>326</v>
       </c>
       <c r="D31" s="33" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="E31" s="32" t="s">
         <v>49</v>
       </c>
       <c r="F31" s="32" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="G31" s="4">
         <v>131</v>
@@ -4214,7 +4214,7 @@
       <c r="AJ31" s="19"/>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A32" s="73"/>
+      <c r="A32" s="81"/>
       <c r="B32" s="34">
         <v>29</v>
       </c>
@@ -4222,13 +4222,13 @@
         <v>327</v>
       </c>
       <c r="D32" s="33" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="E32" s="32" t="s">
         <v>51</v>
       </c>
       <c r="F32" s="32" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="G32" s="4">
         <v>101</v>
@@ -4264,7 +4264,7 @@
       <c r="AJ32" s="19"/>
     </row>
     <row r="33" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A33" s="73"/>
+      <c r="A33" s="81"/>
       <c r="B33" s="34">
         <v>30</v>
       </c>
@@ -4272,13 +4272,13 @@
         <v>328</v>
       </c>
       <c r="D33" s="33" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="E33" s="32" t="s">
         <v>42</v>
       </c>
       <c r="F33" s="32" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="G33" s="4">
         <v>59</v>
@@ -4314,7 +4314,7 @@
       <c r="AJ33" s="19"/>
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A34" s="73"/>
+      <c r="A34" s="81"/>
       <c r="B34" s="34">
         <v>31</v>
       </c>
@@ -4322,13 +4322,13 @@
         <v>329</v>
       </c>
       <c r="D34" s="33" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E34" s="32" t="s">
         <v>44</v>
       </c>
       <c r="F34" s="32" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="G34" s="4">
         <v>116</v>
@@ -4364,7 +4364,7 @@
       <c r="AJ34" s="19"/>
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A35" s="73"/>
+      <c r="A35" s="81"/>
       <c r="B35" s="34">
         <v>32</v>
       </c>
@@ -4372,13 +4372,13 @@
         <v>330</v>
       </c>
       <c r="D35" s="33" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="E35" s="32" t="s">
         <v>46</v>
       </c>
       <c r="F35" s="32" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="G35" s="4">
         <v>64</v>
@@ -4414,7 +4414,7 @@
       <c r="AJ35" s="19"/>
     </row>
     <row r="36" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A36" s="73"/>
+      <c r="A36" s="81"/>
       <c r="B36" s="34">
         <v>33</v>
       </c>
@@ -4422,13 +4422,13 @@
         <v>331</v>
       </c>
       <c r="D36" s="33" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="E36" s="32" t="s">
         <v>48</v>
       </c>
       <c r="F36" s="32" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="G36" s="4">
         <v>66</v>
@@ -4464,7 +4464,7 @@
       <c r="AJ36" s="19"/>
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A37" s="73"/>
+      <c r="A37" s="81"/>
       <c r="B37" s="34">
         <v>34</v>
       </c>
@@ -4472,13 +4472,13 @@
         <v>332</v>
       </c>
       <c r="D37" s="33" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="E37" s="32" t="s">
         <v>50</v>
       </c>
       <c r="F37" s="32" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="G37" s="4">
         <v>132</v>
@@ -4514,7 +4514,7 @@
       <c r="AJ37" s="19"/>
     </row>
     <row r="38" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A38" s="74"/>
+      <c r="A38" s="80"/>
       <c r="B38" s="34">
         <v>35</v>
       </c>
@@ -4522,13 +4522,13 @@
         <v>333</v>
       </c>
       <c r="D38" s="33" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="E38" s="32" t="s">
         <v>52</v>
       </c>
       <c r="F38" s="32" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="G38" s="4">
         <v>133</v>
@@ -4602,14 +4602,14 @@
       <c r="AJ39" s="20"/>
     </row>
     <row r="40" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A40" s="75" t="s">
+      <c r="A40" s="78" t="s">
         <v>336</v>
       </c>
       <c r="B40" s="37">
         <v>86</v>
       </c>
       <c r="C40" s="36" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="D40" s="36" t="s">
         <v>54</v>
@@ -4657,7 +4657,7 @@
         <v>87</v>
       </c>
       <c r="C41" s="36" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D41" s="36" t="s">
         <v>56</v>
@@ -4705,7 +4705,7 @@
         <v>88</v>
       </c>
       <c r="C42" s="36" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D42" s="36" t="s">
         <v>58</v>
@@ -4753,7 +4753,7 @@
         <v>89</v>
       </c>
       <c r="C43" s="36" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D43" s="36" t="s">
         <v>60</v>
@@ -4801,7 +4801,7 @@
         <v>90</v>
       </c>
       <c r="C44" s="36" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D44" s="36" t="s">
         <v>62</v>
@@ -4849,7 +4849,7 @@
         <v>91</v>
       </c>
       <c r="C45" s="36" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D45" s="36" t="s">
         <v>64</v>
@@ -4930,14 +4930,14 @@
       <c r="AJ46" s="19"/>
     </row>
     <row r="47" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="72" t="s">
+      <c r="A47" s="79" t="s">
         <v>335</v>
       </c>
       <c r="B47" s="34">
         <v>75</v>
       </c>
       <c r="C47" s="33" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D47" s="33" t="s">
         <v>66</v>
@@ -4946,7 +4946,7 @@
         <v>65</v>
       </c>
       <c r="F47" s="32" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="G47" s="4">
         <v>135</v>
@@ -4982,12 +4982,12 @@
       <c r="AJ47" s="19"/>
     </row>
     <row r="48" spans="1:36" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="73"/>
+      <c r="A48" s="81"/>
       <c r="B48" s="34">
         <v>93</v>
       </c>
       <c r="C48" s="33" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D48" s="33" t="s">
         <v>68</v>
@@ -4996,7 +4996,7 @@
         <v>67</v>
       </c>
       <c r="F48" s="32" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="G48" s="4">
         <v>88</v>
@@ -5032,12 +5032,12 @@
       <c r="AJ48" s="19"/>
     </row>
     <row r="49" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A49" s="73"/>
+      <c r="A49" s="81"/>
       <c r="B49" s="34">
         <v>76</v>
       </c>
       <c r="C49" s="33" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D49" s="33" t="s">
         <v>70</v>
@@ -5046,7 +5046,7 @@
         <v>69</v>
       </c>
       <c r="F49" s="32" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="G49" s="4">
         <v>14</v>
@@ -5082,12 +5082,12 @@
       <c r="AJ49" s="19"/>
     </row>
     <row r="50" spans="1:36" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="74"/>
+      <c r="A50" s="80"/>
       <c r="B50" s="34">
         <v>95</v>
       </c>
       <c r="C50" s="33" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D50" s="33" t="s">
         <v>72</v>
@@ -5096,7 +5096,7 @@
         <v>71</v>
       </c>
       <c r="F50" s="32" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="G50" s="4">
         <v>77</v>
@@ -5170,7 +5170,7 @@
       <c r="AJ51" s="20"/>
     </row>
     <row r="52" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A52" s="75" t="s">
+      <c r="A52" s="78" t="s">
         <v>73</v>
       </c>
       <c r="B52" s="37">
@@ -5273,7 +5273,7 @@
         <v>71</v>
       </c>
       <c r="C54" s="36" t="s">
-        <v>348</v>
+        <v>622</v>
       </c>
       <c r="D54" s="36" t="s">
         <v>79</v>
@@ -5417,7 +5417,7 @@
         <v>25</v>
       </c>
       <c r="C57" s="36" t="s">
-        <v>349</v>
+        <v>623</v>
       </c>
       <c r="D57" s="36" t="s">
         <v>85</v>
@@ -5498,14 +5498,14 @@
       <c r="AJ58" s="19"/>
     </row>
     <row r="59" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="72" t="s">
-        <v>625</v>
+      <c r="A59" s="79" t="s">
+        <v>621</v>
       </c>
       <c r="B59" s="34">
         <v>48</v>
       </c>
       <c r="C59" s="33" t="s">
-        <v>343</v>
+        <v>625</v>
       </c>
       <c r="D59" s="33" t="s">
         <v>98</v>
@@ -5548,12 +5548,12 @@
       <c r="AJ59" s="19"/>
     </row>
     <row r="60" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A60" s="74"/>
+      <c r="A60" s="80"/>
       <c r="B60" s="34">
         <v>49</v>
       </c>
       <c r="C60" s="33" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D60" s="33" t="s">
         <v>100</v>
@@ -5598,14 +5598,14 @@
       <c r="AJ60" s="19"/>
     </row>
     <row r="61" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A61" s="72" t="s">
+      <c r="A61" s="79" t="s">
         <v>86</v>
       </c>
       <c r="B61" s="34">
         <v>50</v>
       </c>
       <c r="C61" s="33" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D61" s="33" t="s">
         <v>88</v>
@@ -5648,7 +5648,7 @@
       <c r="AJ61" s="19"/>
     </row>
     <row r="62" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A62" s="73"/>
+      <c r="A62" s="81"/>
       <c r="B62" s="34">
         <v>51</v>
       </c>
@@ -5696,7 +5696,7 @@
       <c r="AJ62" s="19"/>
     </row>
     <row r="63" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A63" s="73"/>
+      <c r="A63" s="81"/>
       <c r="B63" s="34">
         <v>52</v>
       </c>
@@ -5744,12 +5744,12 @@
       <c r="AJ63" s="19"/>
     </row>
     <row r="64" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A64" s="73"/>
+      <c r="A64" s="81"/>
       <c r="B64" s="34">
         <v>53</v>
       </c>
       <c r="C64" s="33" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D64" s="33" t="s">
         <v>94</v>
@@ -5792,12 +5792,12 @@
       <c r="AJ64" s="19"/>
     </row>
     <row r="65" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A65" s="74"/>
+      <c r="A65" s="80"/>
       <c r="B65" s="34">
         <v>54</v>
       </c>
       <c r="C65" s="33" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D65" s="33" t="s">
         <v>96</v>
@@ -5878,7 +5878,7 @@
       <c r="AJ66" s="19"/>
     </row>
     <row r="67" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A67" s="72" t="s">
+      <c r="A67" s="79" t="s">
         <v>102</v>
       </c>
       <c r="B67" s="34">
@@ -5930,7 +5930,7 @@
       <c r="AJ67" s="19"/>
     </row>
     <row r="68" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A68" s="73"/>
+      <c r="A68" s="81"/>
       <c r="B68" s="34">
         <v>1</v>
       </c>
@@ -5980,7 +5980,7 @@
       <c r="AJ68" s="19"/>
     </row>
     <row r="69" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A69" s="73"/>
+      <c r="A69" s="81"/>
       <c r="B69" s="34">
         <v>4</v>
       </c>
@@ -6028,7 +6028,7 @@
       <c r="AJ69" s="19"/>
     </row>
     <row r="70" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A70" s="73"/>
+      <c r="A70" s="81"/>
       <c r="B70" s="34">
         <v>7</v>
       </c>
@@ -6076,7 +6076,7 @@
       <c r="AJ70" s="19"/>
     </row>
     <row r="71" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A71" s="73"/>
+      <c r="A71" s="81"/>
       <c r="B71" s="34">
         <v>11</v>
       </c>
@@ -6124,7 +6124,7 @@
       <c r="AJ71" s="19"/>
     </row>
     <row r="72" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A72" s="73"/>
+      <c r="A72" s="81"/>
       <c r="B72" s="34">
         <v>12</v>
       </c>
@@ -6172,7 +6172,7 @@
       <c r="AJ72" s="19"/>
     </row>
     <row r="73" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A73" s="73"/>
+      <c r="A73" s="81"/>
       <c r="B73" s="34">
         <v>8</v>
       </c>
@@ -6220,7 +6220,7 @@
       <c r="AJ73" s="19"/>
     </row>
     <row r="74" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A74" s="73"/>
+      <c r="A74" s="81"/>
       <c r="B74" s="34">
         <v>3</v>
       </c>
@@ -6268,7 +6268,7 @@
       <c r="AJ74" s="19"/>
     </row>
     <row r="75" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A75" s="73"/>
+      <c r="A75" s="81"/>
       <c r="B75" s="34">
         <v>5</v>
       </c>
@@ -6316,7 +6316,7 @@
       <c r="AJ75" s="19"/>
     </row>
     <row r="76" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A76" s="73"/>
+      <c r="A76" s="81"/>
       <c r="B76" s="34">
         <v>6</v>
       </c>
@@ -6364,7 +6364,7 @@
       <c r="AJ76" s="19"/>
     </row>
     <row r="77" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A77" s="73"/>
+      <c r="A77" s="81"/>
       <c r="B77" s="34">
         <v>9</v>
       </c>
@@ -6412,7 +6412,7 @@
       <c r="AJ77" s="19"/>
     </row>
     <row r="78" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A78" s="73"/>
+      <c r="A78" s="81"/>
       <c r="B78" s="34">
         <v>2</v>
       </c>
@@ -6460,7 +6460,7 @@
       <c r="AJ78" s="19"/>
     </row>
     <row r="79" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A79" s="73"/>
+      <c r="A79" s="81"/>
       <c r="B79" s="34">
         <v>10</v>
       </c>
@@ -6508,7 +6508,7 @@
       <c r="AJ79" s="19"/>
     </row>
     <row r="80" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A80" s="74"/>
+      <c r="A80" s="80"/>
       <c r="B80" s="34">
         <v>13</v>
       </c>
@@ -6594,7 +6594,7 @@
       <c r="AJ81" s="19"/>
     </row>
     <row r="82" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A82" s="86" t="s">
+      <c r="A82" s="93" t="s">
         <v>138</v>
       </c>
       <c r="B82" s="37">
@@ -6646,7 +6646,7 @@
       <c r="AJ82" s="19"/>
     </row>
     <row r="83" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A83" s="86"/>
+      <c r="A83" s="93"/>
       <c r="B83" s="37">
         <v>56</v>
       </c>
@@ -6694,7 +6694,7 @@
       <c r="AJ83" s="19"/>
     </row>
     <row r="84" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="86"/>
+      <c r="A84" s="93"/>
       <c r="B84" s="37">
         <v>57</v>
       </c>
@@ -6742,7 +6742,7 @@
       <c r="AJ84" s="19"/>
     </row>
     <row r="85" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A85" s="86"/>
+      <c r="A85" s="93"/>
       <c r="B85" s="37">
         <v>58</v>
       </c>
@@ -6792,7 +6792,7 @@
       <c r="AJ85" s="19"/>
     </row>
     <row r="86" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A86" s="86"/>
+      <c r="A86" s="93"/>
       <c r="B86" s="37">
         <v>59</v>
       </c>
@@ -6840,7 +6840,7 @@
       <c r="AJ86" s="19"/>
     </row>
     <row r="87" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A87" s="86"/>
+      <c r="A87" s="93"/>
       <c r="B87" s="37">
         <v>60</v>
       </c>
@@ -6926,7 +6926,7 @@
       <c r="AJ88" s="19"/>
     </row>
     <row r="89" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="72" t="s">
+      <c r="A89" s="79" t="s">
         <v>334</v>
       </c>
       <c r="B89" s="34">
@@ -6976,7 +6976,7 @@
       <c r="AJ89" s="19"/>
     </row>
     <row r="90" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A90" s="73"/>
+      <c r="A90" s="81"/>
       <c r="B90" s="34">
         <v>64</v>
       </c>
@@ -7024,7 +7024,7 @@
       <c r="AJ90" s="19"/>
     </row>
     <row r="91" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A91" s="73"/>
+      <c r="A91" s="81"/>
       <c r="B91" s="34">
         <v>68</v>
       </c>
@@ -7072,7 +7072,7 @@
       <c r="AJ91" s="19"/>
     </row>
     <row r="92" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A92" s="73"/>
+      <c r="A92" s="81"/>
       <c r="B92" s="34">
         <v>66</v>
       </c>
@@ -7120,7 +7120,7 @@
       <c r="AJ92" s="19"/>
     </row>
     <row r="93" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A93" s="73"/>
+      <c r="A93" s="81"/>
       <c r="B93" s="34">
         <v>63</v>
       </c>
@@ -7168,7 +7168,7 @@
       <c r="AJ93" s="19"/>
     </row>
     <row r="94" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A94" s="73"/>
+      <c r="A94" s="81"/>
       <c r="B94" s="34">
         <v>67</v>
       </c>
@@ -7216,7 +7216,7 @@
       <c r="AJ94" s="19"/>
     </row>
     <row r="95" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A95" s="73"/>
+      <c r="A95" s="81"/>
       <c r="B95" s="34">
         <v>61</v>
       </c>
@@ -7264,7 +7264,7 @@
       <c r="AJ95" s="19"/>
     </row>
     <row r="96" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A96" s="74"/>
+      <c r="A96" s="80"/>
       <c r="B96" s="34">
         <v>62</v>
       </c>
@@ -7350,7 +7350,7 @@
       <c r="AJ97" s="19"/>
     </row>
     <row r="98" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A98" s="75" t="s">
+      <c r="A98" s="78" t="s">
         <v>337</v>
       </c>
       <c r="B98" s="47">
@@ -7638,23 +7638,23 @@
       <c r="AJ103" s="19"/>
     </row>
     <row r="104" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A104" s="87" t="s">
+      <c r="A104" s="94" t="s">
         <v>178</v>
       </c>
       <c r="B104" s="54">
         <v>77</v>
       </c>
       <c r="C104" s="53" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D104" s="53" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E104" s="52" t="s">
         <v>177</v>
       </c>
-      <c r="F104" s="84" t="s">
-        <v>354</v>
+      <c r="F104" s="91" t="s">
+        <v>351</v>
       </c>
       <c r="G104" s="4">
         <v>17</v>
@@ -7690,12 +7690,12 @@
       <c r="AJ104" s="19"/>
     </row>
     <row r="105" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A105" s="88"/>
+      <c r="A105" s="95"/>
       <c r="B105" s="55">
         <v>78</v>
       </c>
       <c r="C105" s="56" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D105" s="56" t="s">
         <v>289</v>
@@ -7703,7 +7703,7 @@
       <c r="E105" s="57" t="s">
         <v>176</v>
       </c>
-      <c r="F105" s="85"/>
+      <c r="F105" s="92"/>
       <c r="G105" s="4">
         <v>18</v>
       </c>
@@ -7738,20 +7738,20 @@
       <c r="AJ105" s="19"/>
     </row>
     <row r="106" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A106" s="88"/>
+      <c r="A106" s="95"/>
       <c r="B106" s="55">
         <v>79</v>
       </c>
       <c r="C106" s="56" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D106" s="56" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E106" s="57" t="s">
-        <v>358</v>
-      </c>
-      <c r="F106" s="69" t="s">
+        <v>355</v>
+      </c>
+      <c r="F106" s="82" t="s">
         <v>242</v>
       </c>
       <c r="G106" s="4">
@@ -7788,7 +7788,7 @@
       <c r="AJ106" s="19"/>
     </row>
     <row r="107" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A107" s="88"/>
+      <c r="A107" s="95"/>
       <c r="B107" s="55">
         <v>80</v>
       </c>
@@ -7801,7 +7801,7 @@
       <c r="E107" s="57" t="s">
         <v>241</v>
       </c>
-      <c r="F107" s="70"/>
+      <c r="F107" s="83"/>
       <c r="G107" s="4">
         <v>70</v>
       </c>
@@ -7836,12 +7836,12 @@
       <c r="AJ107" s="19"/>
     </row>
     <row r="108" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A108" s="89"/>
+      <c r="A108" s="96"/>
       <c r="B108" s="55">
         <v>83</v>
       </c>
       <c r="C108" s="56" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D108" s="56" t="s">
         <v>170</v>
@@ -7924,8 +7924,8 @@
       <c r="AJ109" s="19"/>
     </row>
     <row r="110" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A110" s="79" t="s">
-        <v>364</v>
+      <c r="A110" s="86" t="s">
+        <v>360</v>
       </c>
       <c r="B110" s="50">
         <v>92</v>
@@ -7976,12 +7976,12 @@
       <c r="AJ110" s="19"/>
     </row>
     <row r="111" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A111" s="80"/>
+      <c r="A111" s="87"/>
       <c r="B111" s="50">
         <v>94</v>
       </c>
       <c r="C111" s="49" t="s">
-        <v>361</v>
+        <v>624</v>
       </c>
       <c r="D111" s="49" t="s">
         <v>289</v>
@@ -8064,8 +8064,8 @@
       <c r="AJ112" s="19"/>
     </row>
     <row r="113" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A113" s="72" t="s">
-        <v>621</v>
+      <c r="A113" s="79" t="s">
+        <v>617</v>
       </c>
       <c r="B113" s="55">
         <v>81</v>
@@ -8079,7 +8079,7 @@
       <c r="E113" s="57" t="s">
         <v>252</v>
       </c>
-      <c r="F113" s="69" t="s">
+      <c r="F113" s="82" t="s">
         <v>253</v>
       </c>
       <c r="G113" s="4">
@@ -8116,7 +8116,7 @@
       <c r="AJ113" s="19"/>
     </row>
     <row r="114" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A114" s="74"/>
+      <c r="A114" s="80"/>
       <c r="B114" s="55">
         <v>82</v>
       </c>
@@ -8129,7 +8129,7 @@
       <c r="E114" s="57" t="s">
         <v>254</v>
       </c>
-      <c r="F114" s="70"/>
+      <c r="F114" s="83"/>
       <c r="G114" s="4">
         <v>87</v>
       </c>
@@ -8203,7 +8203,7 @@
     </row>
     <row r="116" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A116" s="51" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B116" s="50">
         <v>84</v>
@@ -8255,22 +8255,22 @@
     </row>
     <row r="117" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A117" s="51" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B117" s="50">
         <v>85</v>
       </c>
       <c r="C117" s="49" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D117" s="49" t="s">
         <v>169</v>
       </c>
       <c r="E117" s="48" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="F117" s="48" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="G117" s="4">
         <v>55</v>
@@ -8558,7 +8558,7 @@
       <c r="AJ123" s="19"/>
     </row>
     <row r="124" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="81" t="s">
+      <c r="A124" s="88" t="s">
         <v>244</v>
       </c>
       <c r="B124" s="46"/>
@@ -8604,7 +8604,7 @@
       <c r="AJ124" s="19"/>
     </row>
     <row r="125" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A125" s="82"/>
+      <c r="A125" s="89"/>
       <c r="B125" s="46"/>
       <c r="C125" s="44"/>
       <c r="D125" s="44" t="s">
@@ -8648,7 +8648,7 @@
       <c r="AJ125" s="19"/>
     </row>
     <row r="126" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A126" s="82"/>
+      <c r="A126" s="89"/>
       <c r="B126" s="46"/>
       <c r="C126" s="44"/>
       <c r="D126" s="44" t="s">
@@ -8692,7 +8692,7 @@
       <c r="AJ126" s="19"/>
     </row>
     <row r="127" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A127" s="82"/>
+      <c r="A127" s="89"/>
       <c r="B127" s="46"/>
       <c r="C127" s="44"/>
       <c r="D127" s="44" t="s">
@@ -8736,7 +8736,7 @@
       <c r="AJ127" s="19"/>
     </row>
     <row r="128" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A128" s="82"/>
+      <c r="A128" s="89"/>
       <c r="B128" s="46"/>
       <c r="C128" s="44"/>
       <c r="D128" s="44" t="s">
@@ -8780,7 +8780,7 @@
       <c r="AJ128" s="19"/>
     </row>
     <row r="129" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A129" s="82"/>
+      <c r="A129" s="89"/>
       <c r="B129" s="46"/>
       <c r="C129" s="44"/>
       <c r="D129" s="44" t="s">
@@ -8824,7 +8824,7 @@
       <c r="AJ129" s="19"/>
     </row>
     <row r="130" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A130" s="82"/>
+      <c r="A130" s="89"/>
       <c r="B130" s="46"/>
       <c r="C130" s="44"/>
       <c r="D130" s="44" t="s">
@@ -8868,7 +8868,7 @@
       <c r="AJ130" s="19"/>
     </row>
     <row r="131" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A131" s="82"/>
+      <c r="A131" s="89"/>
       <c r="B131" s="46"/>
       <c r="C131" s="44"/>
       <c r="D131" s="44" t="s">
@@ -8912,7 +8912,7 @@
       <c r="AJ131" s="19"/>
     </row>
     <row r="132" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A132" s="82"/>
+      <c r="A132" s="89"/>
       <c r="B132" s="46"/>
       <c r="C132" s="44"/>
       <c r="D132" s="44" t="s">
@@ -8956,7 +8956,7 @@
       <c r="AJ132" s="19"/>
     </row>
     <row r="133" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A133" s="82"/>
+      <c r="A133" s="89"/>
       <c r="B133" s="46"/>
       <c r="C133" s="44"/>
       <c r="D133" s="44" t="s">
@@ -9000,7 +9000,7 @@
       <c r="AJ133" s="19"/>
     </row>
     <row r="134" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A134" s="82"/>
+      <c r="A134" s="89"/>
       <c r="B134" s="46"/>
       <c r="C134" s="44"/>
       <c r="D134" s="44" t="s">
@@ -9044,7 +9044,7 @@
       <c r="AJ134" s="19"/>
     </row>
     <row r="135" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A135" s="82"/>
+      <c r="A135" s="89"/>
       <c r="B135" s="46"/>
       <c r="C135" s="44"/>
       <c r="D135" s="44" t="s">
@@ -9088,7 +9088,7 @@
       <c r="AJ135" s="19"/>
     </row>
     <row r="136" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A136" s="82"/>
+      <c r="A136" s="89"/>
       <c r="B136" s="46"/>
       <c r="C136" s="44"/>
       <c r="D136" s="44" t="s">
@@ -9132,7 +9132,7 @@
       <c r="AJ136" s="19"/>
     </row>
     <row r="137" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A137" s="82"/>
+      <c r="A137" s="89"/>
       <c r="B137" s="46"/>
       <c r="C137" s="44"/>
       <c r="D137" s="44" t="s">
@@ -9176,7 +9176,7 @@
       <c r="AJ137" s="19"/>
     </row>
     <row r="138" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A138" s="82"/>
+      <c r="A138" s="89"/>
       <c r="B138" s="46"/>
       <c r="C138" s="44"/>
       <c r="D138" s="44" t="s">
@@ -9220,7 +9220,7 @@
       <c r="AJ138" s="19"/>
     </row>
     <row r="139" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A139" s="82"/>
+      <c r="A139" s="89"/>
       <c r="B139" s="46"/>
       <c r="C139" s="44"/>
       <c r="D139" s="44" t="s">
@@ -9266,7 +9266,7 @@
       <c r="AJ139" s="19"/>
     </row>
     <row r="140" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A140" s="82"/>
+      <c r="A140" s="89"/>
       <c r="B140" s="46"/>
       <c r="C140" s="44"/>
       <c r="D140" s="44" t="s">
@@ -9312,7 +9312,7 @@
       <c r="AJ140" s="19"/>
     </row>
     <row r="141" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A141" s="82"/>
+      <c r="A141" s="89"/>
       <c r="B141" s="46"/>
       <c r="C141" s="44"/>
       <c r="D141" s="44" t="s">
@@ -9358,7 +9358,7 @@
       <c r="AJ141" s="19"/>
     </row>
     <row r="142" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A142" s="82"/>
+      <c r="A142" s="89"/>
       <c r="B142" s="46"/>
       <c r="C142" s="44"/>
       <c r="D142" s="44" t="s">
@@ -9404,7 +9404,7 @@
       <c r="AJ142" s="19"/>
     </row>
     <row r="143" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A143" s="82"/>
+      <c r="A143" s="89"/>
       <c r="B143" s="46"/>
       <c r="C143" s="44"/>
       <c r="D143" s="44" t="s">
@@ -9450,7 +9450,7 @@
       <c r="AJ143" s="19"/>
     </row>
     <row r="144" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A144" s="82"/>
+      <c r="A144" s="89"/>
       <c r="B144" s="46"/>
       <c r="C144" s="44"/>
       <c r="D144" s="44" t="s">
@@ -9494,7 +9494,7 @@
       <c r="AJ144" s="19"/>
     </row>
     <row r="145" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A145" s="82"/>
+      <c r="A145" s="89"/>
       <c r="B145" s="46"/>
       <c r="C145" s="44"/>
       <c r="D145" s="44" t="s">
@@ -9538,7 +9538,7 @@
       <c r="AJ145" s="19"/>
     </row>
     <row r="146" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A146" s="82"/>
+      <c r="A146" s="89"/>
       <c r="B146" s="46"/>
       <c r="C146" s="44"/>
       <c r="D146" s="44" t="s">
@@ -9582,7 +9582,7 @@
       <c r="AJ146" s="19"/>
     </row>
     <row r="147" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A147" s="82"/>
+      <c r="A147" s="89"/>
       <c r="B147" s="46"/>
       <c r="C147" s="44"/>
       <c r="D147" s="44" t="s">
@@ -9626,7 +9626,7 @@
       <c r="AJ147" s="19"/>
     </row>
     <row r="148" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A148" s="82"/>
+      <c r="A148" s="89"/>
       <c r="B148" s="46"/>
       <c r="C148" s="44"/>
       <c r="D148" s="44" t="s">
@@ -9672,7 +9672,7 @@
       <c r="AJ148" s="19"/>
     </row>
     <row r="149" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A149" s="82"/>
+      <c r="A149" s="89"/>
       <c r="B149" s="46"/>
       <c r="C149" s="44"/>
       <c r="D149" s="44" t="s">
@@ -9716,7 +9716,7 @@
       <c r="AJ149" s="19"/>
     </row>
     <row r="150" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A150" s="82"/>
+      <c r="A150" s="89"/>
       <c r="B150" s="46"/>
       <c r="C150" s="44"/>
       <c r="D150" s="44" t="s">
@@ -9762,7 +9762,7 @@
       <c r="AJ150" s="19"/>
     </row>
     <row r="151" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A151" s="82"/>
+      <c r="A151" s="89"/>
       <c r="B151" s="46"/>
       <c r="C151" s="44"/>
       <c r="D151" s="44" t="s">
@@ -9808,7 +9808,7 @@
       <c r="AJ151" s="19"/>
     </row>
     <row r="152" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A152" s="82"/>
+      <c r="A152" s="89"/>
       <c r="B152" s="46"/>
       <c r="C152" s="44"/>
       <c r="D152" s="44" t="s">
@@ -9854,7 +9854,7 @@
       <c r="AJ152" s="19"/>
     </row>
     <row r="153" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A153" s="82"/>
+      <c r="A153" s="89"/>
       <c r="B153" s="46"/>
       <c r="C153" s="44"/>
       <c r="D153" s="44" t="s">
@@ -9900,7 +9900,7 @@
       <c r="AJ153" s="19"/>
     </row>
     <row r="154" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A154" s="82"/>
+      <c r="A154" s="89"/>
       <c r="B154" s="46"/>
       <c r="C154" s="44"/>
       <c r="D154" s="44" t="s">
@@ -9944,7 +9944,7 @@
       <c r="AJ154" s="19"/>
     </row>
     <row r="155" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A155" s="82"/>
+      <c r="A155" s="89"/>
       <c r="B155" s="46"/>
       <c r="C155" s="44"/>
       <c r="D155" s="44" t="s">
@@ -9988,7 +9988,7 @@
       <c r="AJ155" s="19"/>
     </row>
     <row r="156" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A156" s="82"/>
+      <c r="A156" s="89"/>
       <c r="B156" s="46"/>
       <c r="C156" s="44"/>
       <c r="D156" s="44" t="s">
@@ -10032,7 +10032,7 @@
       <c r="AJ156" s="19"/>
     </row>
     <row r="157" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A157" s="82"/>
+      <c r="A157" s="89"/>
       <c r="B157" s="46"/>
       <c r="C157" s="44"/>
       <c r="D157" s="44" t="s">
@@ -10076,7 +10076,7 @@
       <c r="AJ157" s="19"/>
     </row>
     <row r="158" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A158" s="82"/>
+      <c r="A158" s="89"/>
       <c r="B158" s="46"/>
       <c r="C158" s="44"/>
       <c r="D158" s="44" t="s">
@@ -10120,7 +10120,7 @@
       <c r="AJ158" s="19"/>
     </row>
     <row r="159" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A159" s="82"/>
+      <c r="A159" s="89"/>
       <c r="B159" s="46"/>
       <c r="C159" s="44"/>
       <c r="D159" s="44" t="s">
@@ -10164,7 +10164,7 @@
       <c r="AJ159" s="19"/>
     </row>
     <row r="160" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A160" s="82"/>
+      <c r="A160" s="89"/>
       <c r="B160" s="46"/>
       <c r="C160" s="44"/>
       <c r="D160" s="44" t="s">
@@ -10208,7 +10208,7 @@
       <c r="AJ160" s="19"/>
     </row>
     <row r="161" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A161" s="82"/>
+      <c r="A161" s="89"/>
       <c r="B161" s="46"/>
       <c r="C161" s="44"/>
       <c r="D161" s="44" t="s">
@@ -10252,7 +10252,7 @@
       <c r="AJ161" s="19"/>
     </row>
     <row r="162" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A162" s="82"/>
+      <c r="A162" s="89"/>
       <c r="B162" s="46"/>
       <c r="C162" s="44"/>
       <c r="D162" s="44" t="s">
@@ -10298,7 +10298,7 @@
       <c r="AJ162" s="19"/>
     </row>
     <row r="163" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A163" s="82"/>
+      <c r="A163" s="89"/>
       <c r="B163" s="46"/>
       <c r="C163" s="44"/>
       <c r="D163" s="44" t="s">
@@ -10344,7 +10344,7 @@
       <c r="AJ163" s="19"/>
     </row>
     <row r="164" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A164" s="82"/>
+      <c r="A164" s="89"/>
       <c r="B164" s="46"/>
       <c r="C164" s="44"/>
       <c r="D164" s="44" t="s">
@@ -10390,7 +10390,7 @@
       <c r="AJ164" s="19"/>
     </row>
     <row r="165" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A165" s="82"/>
+      <c r="A165" s="89"/>
       <c r="B165" s="46"/>
       <c r="C165" s="44"/>
       <c r="D165" s="44"/>
@@ -10428,7 +10428,7 @@
       <c r="AJ165" s="19"/>
     </row>
     <row r="166" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A166" s="82"/>
+      <c r="A166" s="89"/>
       <c r="B166" s="46"/>
       <c r="C166" s="44"/>
       <c r="D166" s="44" t="s">
@@ -10470,7 +10470,7 @@
       <c r="AJ166" s="19"/>
     </row>
     <row r="167" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A167" s="83"/>
+      <c r="A167" s="90"/>
       <c r="B167" s="46"/>
       <c r="C167" s="44"/>
       <c r="D167" s="44"/>
@@ -10546,7 +10546,7 @@
       <c r="AJ168" s="19"/>
     </row>
     <row r="169" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A169" s="71" t="s">
+      <c r="A169" s="84" t="s">
         <v>243</v>
       </c>
       <c r="B169" s="46"/>
@@ -10594,7 +10594,7 @@
       <c r="AJ169" s="19"/>
     </row>
     <row r="170" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A170" s="71"/>
+      <c r="A170" s="84"/>
       <c r="B170" s="46"/>
       <c r="C170" s="44"/>
       <c r="D170" s="44" t="s">
@@ -10640,7 +10640,7 @@
       <c r="AJ170" s="19"/>
     </row>
     <row r="171" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A171" s="71"/>
+      <c r="A171" s="84"/>
       <c r="B171" s="46"/>
       <c r="C171" s="44"/>
       <c r="D171" s="44" t="s">
@@ -10686,7 +10686,7 @@
       <c r="AJ171" s="19"/>
     </row>
     <row r="172" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A172" s="71"/>
+      <c r="A172" s="84"/>
       <c r="B172" s="46"/>
       <c r="C172" s="44"/>
       <c r="D172" s="44" t="s">
@@ -10737,7 +10737,7 @@
       <c r="C173" s="40"/>
       <c r="D173" s="40"/>
       <c r="E173" s="39"/>
-      <c r="F173" s="96"/>
+      <c r="F173" s="75"/>
       <c r="G173" s="2"/>
       <c r="H173" s="19"/>
       <c r="I173" s="19"/>
@@ -16780,13 +16780,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A98:A102"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="A61:A65"/>
-    <mergeCell ref="A89:A96"/>
-    <mergeCell ref="A40:A45"/>
-    <mergeCell ref="A67:A80"/>
     <mergeCell ref="F113:F114"/>
     <mergeCell ref="F106:F107"/>
     <mergeCell ref="A169:A172"/>
@@ -16802,6 +16795,13 @@
     <mergeCell ref="A82:A87"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A104:A108"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A98:A102"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="A61:A65"/>
+    <mergeCell ref="A89:A96"/>
+    <mergeCell ref="A40:A45"/>
+    <mergeCell ref="A67:A80"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="62" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -16829,25 +16829,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B1" s="65" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="C1" s="65" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="D1" s="65" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="E1" s="65" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F1" s="65" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="G1" s="65" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -16858,7 +16858,7 @@
         <v>74</v>
       </c>
       <c r="D2" s="65" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -16869,10 +16869,10 @@
         <v>76</v>
       </c>
       <c r="D3" s="65" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="F3" s="65" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="G3" s="65">
         <v>1</v>
@@ -16883,13 +16883,13 @@
         <v>58</v>
       </c>
       <c r="B4" s="65" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D4" s="65" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="F4" s="65" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G4" s="65">
         <v>2</v>
@@ -16900,13 +16900,13 @@
         <v>62</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="D5" s="65" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="F5" s="65" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="G5" s="65">
         <v>3</v>
@@ -16917,13 +16917,13 @@
         <v>60</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="D6" s="65" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="F6" s="65" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="G6" s="65">
         <v>2</v>
@@ -16934,13 +16934,13 @@
         <v>8</v>
       </c>
       <c r="B7" s="65" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D7" s="65" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="F7" s="65" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="G7" s="65">
         <v>1</v>
@@ -16951,10 +16951,10 @@
         <v>291</v>
       </c>
       <c r="B8" s="65" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="D8" s="65" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="F8" s="65" t="s">
         <v>189</v>
@@ -16968,13 +16968,13 @@
         <v>137</v>
       </c>
       <c r="B9" s="65" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D9" s="65" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="F9" s="65" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="G9" s="65">
         <v>1</v>
@@ -16985,13 +16985,13 @@
         <v>104</v>
       </c>
       <c r="B10" s="65" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="D10" s="65" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="F10" s="65" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="G10" s="65">
         <v>1</v>
@@ -17002,10 +17002,10 @@
         <v>106</v>
       </c>
       <c r="B11" s="65" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="D11" s="65" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -17013,13 +17013,13 @@
         <v>142</v>
       </c>
       <c r="B12" s="65" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D12" s="65" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="F12" s="65" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="G12" s="65">
         <v>1</v>
@@ -17030,13 +17030,13 @@
         <v>140</v>
       </c>
       <c r="B13" s="65" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D13" s="65" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="F13" s="65" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="G13" s="65">
         <v>1</v>
@@ -17047,13 +17047,13 @@
         <v>148</v>
       </c>
       <c r="B14" s="65" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D14" s="65" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="F14" s="65" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="G14" s="65">
         <v>1</v>
@@ -17064,10 +17064,10 @@
         <v>146</v>
       </c>
       <c r="B15" s="65" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -17075,10 +17075,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="65" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -17086,13 +17086,13 @@
         <v>12</v>
       </c>
       <c r="B17" s="65" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="F17" s="65" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="G17" s="65">
         <v>1</v>
@@ -17103,13 +17103,13 @@
         <v>64</v>
       </c>
       <c r="B18" s="65" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="D18" s="65" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="F18" s="65" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="G18" s="65">
         <v>2</v>
@@ -17117,13 +17117,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="65" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B19" s="65" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D19" s="65" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -17131,13 +17131,13 @@
         <v>240</v>
       </c>
       <c r="B20" s="65" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="D20" s="65" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="F20" s="65" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="G20" s="65">
         <v>1</v>
@@ -17151,7 +17151,7 @@
         <v>34</v>
       </c>
       <c r="D21" s="65" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -17162,7 +17162,7 @@
         <v>32</v>
       </c>
       <c r="D22" s="65" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -17173,7 +17173,7 @@
         <v>36</v>
       </c>
       <c r="D23" s="65" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -17184,10 +17184,10 @@
         <v>38</v>
       </c>
       <c r="D24" s="65" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="F24" s="65" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="G24" s="65">
         <v>2</v>
@@ -17201,10 +17201,10 @@
         <v>28</v>
       </c>
       <c r="D25" s="65" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="F25" s="65" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="G25" s="65">
         <v>2</v>
@@ -17218,10 +17218,10 @@
         <v>30</v>
       </c>
       <c r="D26" s="65" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="F26" s="65" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="G26" s="65">
         <v>2</v>
@@ -17235,7 +17235,7 @@
         <v>338</v>
       </c>
       <c r="D27" s="65" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -17246,7 +17246,7 @@
         <v>339</v>
       </c>
       <c r="D28" s="65" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -17254,13 +17254,13 @@
         <v>133</v>
       </c>
       <c r="B29" s="65" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D29" s="65" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="F29" s="65" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="G29" s="65">
         <v>1</v>
@@ -17271,13 +17271,13 @@
         <v>131</v>
       </c>
       <c r="B30" s="65" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="D30" s="65" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="F30" s="65" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="G30" s="65">
         <v>1</v>
@@ -17288,52 +17288,52 @@
         <v>263</v>
       </c>
       <c r="B31" s="65" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="D31" s="65" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="65" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B32" s="65" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="D32" s="65" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="65" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B33" s="65" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D33" s="65" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="65" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="67" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="67" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="67" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
   </sheetData>
@@ -17362,25 +17362,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B1" s="65" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="C1" s="65" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="D1" s="65" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="E1" s="65" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F1" s="65" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="G1" s="65" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -17388,13 +17388,13 @@
         <v>152</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="C2" s="65">
         <v>1</v>
       </c>
       <c r="D2" s="65" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="E2" s="65">
         <v>2</v>
@@ -17405,13 +17405,13 @@
         <v>165</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="C3" s="65">
         <v>1</v>
       </c>
       <c r="D3" s="65" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="E3" s="65">
         <v>2</v>
@@ -17422,13 +17422,13 @@
         <v>167</v>
       </c>
       <c r="B4" s="65" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C4" s="65">
         <v>1</v>
       </c>
       <c r="D4" s="65" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="E4" s="65">
         <v>2</v>
@@ -17439,13 +17439,13 @@
         <v>111</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C5" s="65">
         <v>1</v>
       </c>
       <c r="D5" s="65" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="E5" s="65">
         <v>2</v>
@@ -17456,13 +17456,13 @@
         <v>144</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="C6" s="65">
         <v>1</v>
       </c>
       <c r="D6" s="65" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="E6" s="65">
         <v>2</v>
@@ -17473,13 +17473,13 @@
         <v>100</v>
       </c>
       <c r="B7" s="65" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C7" s="65">
         <v>1</v>
       </c>
       <c r="D7" s="65" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="E7" s="65">
         <v>2</v>
@@ -17490,13 +17490,13 @@
         <v>24</v>
       </c>
       <c r="B8" s="65" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C8" s="65">
         <v>1</v>
       </c>
       <c r="D8" s="65" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E8" s="65">
         <v>2</v>
@@ -17507,13 +17507,13 @@
         <v>150</v>
       </c>
       <c r="B9" s="65" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C9" s="65">
         <v>1</v>
       </c>
       <c r="D9" s="65" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E9" s="65">
         <v>2</v>
@@ -17524,13 +17524,13 @@
         <v>88</v>
       </c>
       <c r="B10" s="65" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="C10" s="65">
         <v>1</v>
       </c>
       <c r="D10" s="65" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="E10" s="65">
         <v>2</v>
@@ -17541,13 +17541,13 @@
         <v>269</v>
       </c>
       <c r="B11" s="65" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="C11" s="65">
         <v>1</v>
       </c>
       <c r="D11" s="65" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="E11" s="65">
         <v>2</v>
@@ -17561,7 +17561,7 @@
         <v>270</v>
       </c>
       <c r="D12" s="65" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -17572,7 +17572,7 @@
         <v>272</v>
       </c>
       <c r="D13" s="65" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -17580,13 +17580,13 @@
         <v>251</v>
       </c>
       <c r="B14" s="65" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D14" s="65" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="F14" s="65" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="G14" s="65">
         <v>3</v>
@@ -17597,13 +17597,13 @@
         <v>255</v>
       </c>
       <c r="B15" s="65" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="F15" s="65" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="G15" s="65">
         <v>3</v>
@@ -17617,7 +17617,7 @@
         <v>80</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -17628,10 +17628,10 @@
         <v>82</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="F17" s="65" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="G17" s="65">
         <v>4</v>
@@ -17642,10 +17642,10 @@
         <v>72</v>
       </c>
       <c r="B18" s="65" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="D18" s="65" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="F18" s="65" t="s">
         <v>71</v>
@@ -17659,13 +17659,13 @@
         <v>68</v>
       </c>
       <c r="B19" s="65" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="D19" s="65" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="F19" s="65" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="G19" s="65">
         <v>3</v>
@@ -17676,13 +17676,13 @@
         <v>56</v>
       </c>
       <c r="B20" s="65" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D20" s="65" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="F20" s="65" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="G20" s="65">
         <v>3</v>
@@ -17693,13 +17693,13 @@
         <v>54</v>
       </c>
       <c r="B21" s="65" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="D21" s="65" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="F21" s="65" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="G21" s="65">
         <v>3</v>
@@ -17710,13 +17710,13 @@
         <v>256</v>
       </c>
       <c r="B22" s="65" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="D22" s="65" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="F22" s="65" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="G22" s="65">
         <v>3</v>
@@ -17727,13 +17727,13 @@
         <v>170</v>
       </c>
       <c r="B23" s="65" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D23" s="65" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="F23" s="65" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G23" s="65">
         <v>4</v>
@@ -17744,10 +17744,10 @@
         <v>158</v>
       </c>
       <c r="B24" s="65" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D24" s="65" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -17755,13 +17755,13 @@
         <v>161</v>
       </c>
       <c r="B25" s="65" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D25" s="65" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="F25" s="65" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="G25" s="65">
         <v>6</v>
@@ -17772,10 +17772,10 @@
         <v>277</v>
       </c>
       <c r="B26" s="65" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="D26" s="65" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -17783,10 +17783,10 @@
         <v>129</v>
       </c>
       <c r="B27" s="65" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D27" s="65" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -17794,13 +17794,13 @@
         <v>121</v>
       </c>
       <c r="B28" s="65" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="D28" s="65" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="F28" s="65" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="G28" s="65">
         <v>6</v>
@@ -17811,10 +17811,10 @@
         <v>154</v>
       </c>
       <c r="B29" s="65" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="D29" s="65" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -17822,7 +17822,7 @@
         <v>190</v>
       </c>
       <c r="B30" s="65" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -17830,7 +17830,7 @@
         <v>193</v>
       </c>
       <c r="B31" s="65" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -17838,7 +17838,7 @@
         <v>195</v>
       </c>
       <c r="B32" s="65" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -17846,27 +17846,27 @@
         <v>200</v>
       </c>
       <c r="B33" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="65" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" s="67" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B37" s="67" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38" s="66" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="C38" s="66"/>
       <c r="D38" s="66"/>
@@ -17878,17 +17878,17 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B39" s="67" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B40" s="67" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B41" s="67" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -17917,25 +17917,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B1" s="65" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="C1" s="65" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="D1" s="65" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="E1" s="65" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F1" s="65" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="G1" s="65" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -17943,7 +17943,7 @@
         <v>275</v>
       </c>
       <c r="F2" s="65" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="G2" s="65">
         <v>1</v>
@@ -17956,90 +17956,90 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="65" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B4" s="65" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="D4" s="65" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="65" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="D5" s="65" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="65" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="D6" s="65" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="65" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B7" s="65" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="D7" s="65" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="65" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B8" s="65" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="D8" s="65" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="65" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B9" s="65" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="D9" s="65" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="65" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B10" s="65" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D10" s="65" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="65" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B11" s="65" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="D11" s="65" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -18047,10 +18047,10 @@
         <v>98</v>
       </c>
       <c r="B12" s="65" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="D12" s="65" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -18058,10 +18058,10 @@
         <v>110</v>
       </c>
       <c r="B13" s="65" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="D13" s="65" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -18069,10 +18069,10 @@
         <v>117</v>
       </c>
       <c r="B14" s="65" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="D14" s="65" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -18080,10 +18080,10 @@
         <v>123</v>
       </c>
       <c r="B15" s="65" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -18091,10 +18091,10 @@
         <v>125</v>
       </c>
       <c r="B16" s="65" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -18102,10 +18102,10 @@
         <v>127</v>
       </c>
       <c r="B17" s="65" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -18113,10 +18113,10 @@
         <v>163</v>
       </c>
       <c r="B18" s="65" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="D18" s="65" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -18124,10 +18124,10 @@
         <v>135</v>
       </c>
       <c r="B19" s="65" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="D19" s="65" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -18135,54 +18135,54 @@
         <v>94</v>
       </c>
       <c r="B20" s="65" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="D20" s="65" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="65" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B21" s="65" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="D21" s="65" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="65" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B22" s="65" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="D22" s="65" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="65" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B23" s="65" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="D23" s="65" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="65" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B24" s="65" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="D24" s="65" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -18190,10 +18190,10 @@
         <v>96</v>
       </c>
       <c r="B25" s="65" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="D25" s="65" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -18201,10 +18201,10 @@
         <v>66</v>
       </c>
       <c r="B26" s="65" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="D26" s="65" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -18212,10 +18212,10 @@
         <v>18</v>
       </c>
       <c r="B27" s="65" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="D27" s="65" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -18223,10 +18223,10 @@
         <v>92</v>
       </c>
       <c r="B28" s="65" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="D28" s="65" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -18234,10 +18234,10 @@
         <v>22</v>
       </c>
       <c r="B29" s="65" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="D29" s="65" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -18245,10 +18245,10 @@
         <v>90</v>
       </c>
       <c r="B30" s="65" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="D30" s="65" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -18256,10 +18256,10 @@
         <v>156</v>
       </c>
       <c r="B31" s="65" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="D31" s="65" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -18267,20 +18267,20 @@
         <v>26</v>
       </c>
       <c r="B32" s="65" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="D32" s="65" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="67" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B35" s="67" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
   </sheetData>
@@ -18309,25 +18309,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B1" s="65" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="C1" s="65" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="D1" s="65" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="E1" s="65" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F1" s="65" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="G1" s="65" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -18335,10 +18335,10 @@
         <v>85</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="D2" s="65" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -18346,10 +18346,10 @@
         <v>70</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="D3" s="65" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -18357,10 +18357,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="65" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="D4" s="65" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -18368,21 +18368,21 @@
         <v>79</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="D5" s="65" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="65" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D6" s="65" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -18390,10 +18390,10 @@
         <v>289</v>
       </c>
       <c r="B7" s="65" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="D7" s="65" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -18401,10 +18401,10 @@
         <v>113</v>
       </c>
       <c r="B8" s="65" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="D8" s="65" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -18412,10 +18412,10 @@
         <v>20</v>
       </c>
       <c r="B9" s="65" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="D9" s="65" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -18423,10 +18423,10 @@
         <v>16</v>
       </c>
       <c r="B10" s="65" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="D10" s="65" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -18434,10 +18434,10 @@
         <v>115</v>
       </c>
       <c r="B11" s="65" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="D11" s="65" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -18445,172 +18445,172 @@
         <v>6</v>
       </c>
       <c r="B12" s="65" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="65" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="B13" s="65" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="65" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="B14" s="65" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="65" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="B15" s="65" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="65" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B16" s="65" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="65" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="B17" s="65" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="65" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="B18" s="65" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="65" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="B19" s="65" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="65" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="B20" s="65" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="65" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="B21" s="65" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="65" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="B22" s="65" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="65" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="B23" s="65" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="65" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="B24" s="65" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="65" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="B25" s="65" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="65" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="B26" s="65" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="65" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="B27" s="65" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="65" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="B28" s="65" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="65" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="B29" s="65" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="65" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="B30" s="65" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="65" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="B31" s="65" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="65" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="B32" s="65" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="67" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
   </sheetData>

</xml_diff>